<commit_message>
Fix 13: Run code again and check code again
</commit_message>
<xml_diff>
--- a/13.paintballgames/extracted_data/13.Data.xlsx
+++ b/13.paintballgames/extracted_data/13.Data.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Upwork\Task01\Multiple_Directories_Web_scraping\13.paintballgames\extracted_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204758FD-EB12-4755-86FF-E015380B87E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="95">
   <si>
     <t>centreName</t>
   </si>
@@ -89,6 +84,12 @@
 						Wisbech PE14 9JY</t>
   </si>
   <si>
+    <t>Essex – Billericay Paintball</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>East London – Upminster Paintball</t>
   </si>
   <si>
@@ -125,6 +126,9 @@
 						 NE47 0BX</t>
   </si>
   <si>
+    <t>Paintball Manchester</t>
+  </si>
+  <si>
     <t>Manchester Paintball</t>
   </si>
   <si>
@@ -155,6 +159,18 @@
 						 PA6 7BP</t>
   </si>
   <si>
+    <t>East Glasgow Paintball</t>
+  </si>
+  <si>
+    <t>Colchester Paintball</t>
+  </si>
+  <si>
+    <t>West London – Gerrards Cross Paintball</t>
+  </si>
+  <si>
+    <t>Tunbridge Wells Paintball</t>
+  </si>
+  <si>
     <t>Surrey – Cobham Paintball</t>
   </si>
   <si>
@@ -175,6 +191,12 @@
 						Southampton SO16 0AD</t>
   </si>
   <si>
+    <t>South West London – Effingham Paintball</t>
+  </si>
+  <si>
+    <t>South London – Crawley Paintball</t>
+  </si>
+  <si>
     <t>Sittingbourne Paintball</t>
   </si>
   <si>
@@ -185,6 +207,9 @@
 						Newington ME9 7PX</t>
   </si>
   <si>
+    <t>West London – Reading Paintball</t>
+  </si>
+  <si>
     <t>South East London – Orpington Paintball</t>
   </si>
   <si>
@@ -205,6 +230,9 @@
 						 HP1 2RR</t>
   </si>
   <si>
+    <t>North London – Luton Paintball</t>
+  </si>
+  <si>
     <t>Northampton – Banbury Paintball</t>
   </si>
   <si>
@@ -215,6 +243,9 @@
 						 NN13 5NS</t>
   </si>
   <si>
+    <t>Kent – Westerham Paintball</t>
+  </si>
+  <si>
     <t>Berkshire – Maidenhead Paintball</t>
   </si>
   <si>
@@ -265,6 +296,12 @@
 						 CF15 9QN</t>
   </si>
   <si>
+    <t>Staffordshire Paintball</t>
+  </si>
+  <si>
+    <t>Coventry Paintball</t>
+  </si>
+  <si>
     <t>Birmingham Paintball</t>
   </si>
   <si>
@@ -273,6 +310,9 @@
   <si>
     <t>Cut Throat Lane Birmingham 
 						 B94 6SE</t>
+  </si>
+  <si>
+    <t>Sheffield Paintball</t>
   </si>
   <si>
     <t>Leeds – Wakefield Paintball</t>
@@ -288,8 +328,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -333,19 +373,112 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -653,21 +786,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E56633-5C35-45D3-BBF6-41CEBF813862}">
-  <dimension ref="A1:E24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166f015e-975c-474a-ad64-7365a4f1635a}">
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="42.44140625" customWidth="1"/>
-    <col min="2" max="2" width="49.109375" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="1" max="1" width="42.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="49.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="21.5714285714286" customWidth="1"/>
     <col min="4" max="4" width="70" customWidth="1"/>
-    <col min="5" max="5" width="69.33203125" customWidth="1"/>
+    <col min="5" max="5" width="69.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,7 +817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="12.75">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -701,7 +834,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -718,7 +851,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="12.75">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -735,7 +868,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -752,7 +885,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="12.75">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -763,100 +896,100 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="12.75">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="12.75">
+      <c r="A10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:5" ht="12.75">
+      <c r="A12" t="s">
         <v>38</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -865,100 +998,100 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:5" ht="12.75">
+      <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="12.75">
+      <c r="A16" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="12.75">
+      <c r="A18" t="s">
         <v>48</v>
-      </c>
-      <c r="E14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>59</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -967,112 +1100,350 @@
         <v>7</v>
       </c>
       <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="12.75">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="12.75">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12.75">
+      <c r="A24" t="s">
         <v>60</v>
       </c>
-      <c r="E18" t="s">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="E24" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="2" t="s">
+    </row>
+    <row r="25" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E25" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="26" spans="1:5" ht="12.75">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="E27" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="12.75">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="D29" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E29" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="30" spans="1:5" ht="12.75">
+      <c r="A30" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="31" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E31" s="2" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="12.75">
+      <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="12.75">
+      <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="12.75">
+      <c r="A36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="12.75">
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>